<commit_message>
add headers to excel scheet
</commit_message>
<xml_diff>
--- a/ScrapedInvoiceData.xlsx
+++ b/ScrapedInvoiceData.xlsx
@@ -1,71 +1,105 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
-  </bookViews>
-  <sheets>
-    <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
-  </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+<x:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x15">
+  <x:fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <x:workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
+  <x:bookViews>
+    <x:workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="0" activeTab="0"/>
+  </x:bookViews>
+  <x:sheets>
+    <x:sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
+  </x:sheets>
+  <x:definedNames/>
+  <x:calcPr calcId="162913"/>
+  <x:extLst>
+    <x:ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
-</workbook>
+    </x:ext>
+  </x:extLst>
+</x:workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+  <x:si>
+    <x:t>Company Name</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Customer ID</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Invoice Number</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Total amount</x:t>
+  </x:si>
+</x:sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-  </fonts>
-  <fills count="2">
-    <fill>
-      <patternFill patternType="none"/>
-    </fill>
-    <fill>
-      <patternFill patternType="gray125"/>
-    </fill>
-  </fills>
-  <borders count="1">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-  </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-  </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-  </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-  </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+<x:styleSheet xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac x16r2">
+  <x:numFmts count="1">
+    <x:numFmt numFmtId="0" formatCode=""/>
+  </x:numFmts>
+  <x:fonts count="2" x14ac:knownFonts="1">
+    <x:font>
+      <x:sz val="11"/>
+      <x:color theme="1"/>
+      <x:name val="Calibri"/>
+      <x:family val="2"/>
+      <x:scheme val="minor"/>
+    </x:font>
+    <x:font>
+      <x:vertAlign val="baseline"/>
+      <x:sz val="11"/>
+      <x:color rgb="FF000000"/>
+      <x:name val="Calibri"/>
+      <x:family val="2"/>
+    </x:font>
+  </x:fonts>
+  <x:fills count="2">
+    <x:fill>
+      <x:patternFill patternType="none"/>
+    </x:fill>
+    <x:fill>
+      <x:patternFill patternType="gray125"/>
+    </x:fill>
+  </x:fills>
+  <x:borders count="1">
+    <x:border>
+      <x:left/>
+      <x:right/>
+      <x:top/>
+      <x:bottom/>
+      <x:diagonal/>
+    </x:border>
+  </x:borders>
+  <x:cellStyleXfs count="2">
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+  </x:cellStyleXfs>
+  <x:cellXfs count="2">
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+  </x:cellXfs>
+  <x:cellStyles count="1">
+    <x:cellStyle name="Normal" xfId="0" builtinId="0"/>
+  </x:cellStyles>
+  <x:tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <x:extLst>
+    <x:ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+    </x:ext>
+    <x:ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
       <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
-</styleSheet>
+    </x:ext>
+  </x:extLst>
+</x:styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -330,13 +364,35 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac">
+  <x:sheetPr>
+    <x:outlinePr summaryBelow="1" summaryRight="1"/>
+  </x:sheetPr>
+  <x:dimension ref="A1"/>
+  <x:sheetViews>
+    <x:sheetView tabSelected="1" workbookViewId="0"/>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <x:sheetData>
+    <x:row r="1" spans="1:4">
+      <x:c r="A1" s="1" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="B1" s="1" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C1" s="1" t="s">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="D1" s="1" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+  </x:sheetData>
+  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
+  <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
+  <x:headerFooter/>
+  <x:tableParts count="0"/>
+</x:worksheet>
 </file>
</xml_diff>

<commit_message>
extract logo from pdf
</commit_message>
<xml_diff>
--- a/ScrapedInvoiceData.xlsx
+++ b/ScrapedInvoiceData.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<x:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x15">
-  <x:fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <x:workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
+<x:workbook xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <x:fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
+  <x:workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KatarzynaSzyja\Documents\UiPath\PdfDataScraping\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D5D546A-CB07-4EE0-8902-E3BB8DB59608}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <x:bookViews>
-    <x:workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="0" activeTab="0"/>
+    <x:workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8964" firstSheet="0" activeTab="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </x:bookViews>
   <x:sheets>
     <x:sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -20,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <x:si>
     <x:t>Company Name</x:t>
   </x:si>
@@ -31,13 +37,81 @@
     <x:t>Invoice Number</x:t>
   </x:si>
   <x:si>
-    <x:t>Total amount</x:t>
+    <x:t>Total Amount</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Yakidoo
+</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">609
+</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">3031
+</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">650,00 
+</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">650,00 
+</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Jamia
+</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">97
+</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">925,00 
+</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Mydo
+</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">570
+</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">675,00 
+</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Tagopia
+</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">907
+</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">1 825,00 
+</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Fliptune
+</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">346
+</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">1 475,00 
+</x:t>
   </x:si>
 </x:sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<x:styleSheet xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac x16r2">
+<x:styleSheet xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac x16r2 xr">
   <x:numFmts count="1">
     <x:numFmt numFmtId="0" formatCode=""/>
   </x:numFmts>
@@ -50,19 +124,24 @@
       <x:scheme val="minor"/>
     </x:font>
     <x:font>
-      <x:vertAlign val="baseline"/>
       <x:sz val="11"/>
       <x:color rgb="FF000000"/>
       <x:name val="Calibri"/>
       <x:family val="2"/>
     </x:font>
   </x:fonts>
-  <x:fills count="2">
+  <x:fills count="3">
     <x:fill>
       <x:patternFill patternType="none"/>
     </x:fill>
     <x:fill>
       <x:patternFill patternType="gray125"/>
+    </x:fill>
+    <x:fill>
+      <x:patternFill patternType="solid">
+        <x:fgColor rgb="FF483D8B"/>
+        <x:bgColor indexed="64"/>
+      </x:patternFill>
     </x:fill>
   </x:fills>
   <x:borders count="1">
@@ -74,21 +153,48 @@
       <x:diagonal/>
     </x:border>
   </x:borders>
-  <x:cellStyleXfs count="2">
+  <x:cellStyleXfs count="7">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="2">
+  <x:cellXfs count="6">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <x:alignment wrapText="1"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
   </x:cellXfs>
   <x:cellStyles count="1">
-    <x:cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <x:cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </x:cellStyles>
   <x:tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <x:extLst>
@@ -364,28 +470,97 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac">
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{00000000-0001-0000-0000-000000000000}" mc:Ignorable="x14ac xr xr2 xr3">
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1"/>
+  <x:dimension ref="A1:D7"/>
   <x:sheetViews>
     <x:sheetView tabSelected="1" workbookViewId="0"/>
   </x:sheetViews>
-  <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <x:sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <x:sheetData>
-    <x:row r="1" spans="1:4">
-      <x:c r="A1" s="1" t="s">
+    <x:row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <x:c r="A1" s="4" t="s">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="B1" s="1" t="s">
+      <x:c r="B1" s="4" t="s">
         <x:v>1</x:v>
       </x:c>
-      <x:c r="C1" s="1" t="s">
+      <x:c r="C1" s="4" t="s">
         <x:v>2</x:v>
       </x:c>
-      <x:c r="D1" s="1" t="s">
+      <x:c r="D1" s="4" t="s">
         <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:4" customFormat="1" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <x:c r="A2" s="5" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="B2" s="5" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="C2" s="5" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="D2" s="5" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:4" customFormat="1" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <x:c r="A3" s="5" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="B3" s="5" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="C3" s="5" t="s">
+        <x:v>8</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:4" customFormat="1" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <x:c r="A4" s="5" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="B4" s="5" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="C4" s="5" t="s">
+        <x:v>11</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:4" customFormat="1" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <x:c r="A5" s="5" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="B5" s="5" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="C5" s="5" t="s">
+        <x:v>14</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:4" customFormat="1" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <x:c r="A6" s="5" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="B6" s="5" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="C6" s="5" t="s">
+        <x:v>17</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:4" customFormat="1" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <x:c r="A7" s="5" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="B7" s="5" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="C7" s="5" t="s">
+        <x:v>20</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>